<commit_message>
Power budget changed mode names
</commit_message>
<xml_diff>
--- a/block-diagrams/power-budget-c3-rf.xlsx
+++ b/block-diagrams/power-budget-c3-rf.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\block-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DDA20A-98E5-426C-BFC3-6FA7B9D88895}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7D934F-623D-4031-B9E6-A40B84C41254}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21200" yWindow="3130" windowWidth="28480" windowHeight="15400" xr2:uid="{95D7E395-C107-4615-8728-3DDA612325FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17620" xr2:uid="{95D7E395-C107-4615-8728-3DDA612325FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>L band Rx</t>
   </si>
@@ -39,12 +39,6 @@
     <t>UHF Rx</t>
   </si>
   <si>
-    <t>UHF Tx beacon</t>
-  </si>
-  <si>
-    <t>UHF Tx telemetry</t>
-  </si>
-  <si>
     <t>Power (mW)</t>
   </si>
   <si>
@@ -67,12 +61,6 @@
   </si>
   <si>
     <t>Efficiency</t>
-  </si>
-  <si>
-    <t>Load Current (mA)</t>
-  </si>
-  <si>
-    <t>Load Power (mW)</t>
   </si>
   <si>
     <t>for 5.0V</t>
@@ -142,6 +130,50 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>Target Current (mA)</t>
+  </si>
+  <si>
+    <t>Target Power (mW)</t>
+  </si>
+  <si>
+    <r>
+      <t>UHF Tx C.W. Beacon</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>UHF Tx AX.25 Beacon</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>(3) PA output at 0.1W</t>
+  </si>
+  <si>
+    <t>(4) PA output at 1.0W</t>
+  </si>
 </sst>
 </file>
 
@@ -152,9 +184,9 @@
     <numFmt numFmtId="165" formatCode="0.0\ &quot;V&quot;"/>
     <numFmt numFmtId="166" formatCode="0\ &quot;min&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;@&quot;\ 0.0\ &quot;V&quot;"/>
-    <numFmt numFmtId="173" formatCode="&quot;for&quot;\ 0.0\ &quot;V&quot;"/>
-    <numFmt numFmtId="176" formatCode="&quot;Vin =&quot;\ 0.0\ &quot;V&quot;"/>
-    <numFmt numFmtId="181" formatCode="&quot;Vin =&quot;\ 0.0&quot;V&quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;for&quot;\ 0.0\ &quot;V&quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot;Vin =&quot;\ 0.0\ &quot;V&quot;"/>
+    <numFmt numFmtId="170" formatCode="&quot;Vin =&quot;\ 0.0&quot;V&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -364,64 +396,64 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -739,15 +771,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DEDEBC-090E-4C01-8C0C-EFA94C7FB141}">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
     <col min="2" max="2" width="9.36328125" customWidth="1"/>
     <col min="3" max="4" width="9.36328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
@@ -775,36 +807,36 @@
   <sheetData>
     <row r="1" spans="1:24" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="F2" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
+        <v>7</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" s="16">
         <v>7.2</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+        <v>8</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:24" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="17">
         <v>90</v>
@@ -815,60 +847,60 @@
       <c r="B5" s="30"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="J6" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="N6" s="31" t="s">
+      <c r="J6" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="N6" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="49"/>
+      <c r="Q6" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="49"/>
+      <c r="W6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="Q6" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="31"/>
-      <c r="W6" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B7" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="B7" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
       <c r="E7"/>
-      <c r="F7" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="K7" s="39">
+      <c r="F7" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="K7" s="37">
         <v>3.3</v>
       </c>
-      <c r="L7" s="37"/>
-      <c r="N7" s="38" t="str">
+      <c r="L7" s="36"/>
+      <c r="N7" s="50" t="str">
         <f>$B$3 &amp; "V ---&gt; " &amp; $K$7 &amp; "V"</f>
         <v>7.2V ---&gt; 3.3V</v>
       </c>
-      <c r="O7" s="38"/>
-      <c r="Q7" s="38" t="str">
+      <c r="O7" s="50"/>
+      <c r="Q7" s="50" t="str">
         <f>$B$3 &amp; "V ---&gt; " &amp; $B$8 &amp; "V"</f>
         <v>7.2V ---&gt; 5V</v>
       </c>
-      <c r="R7" s="38"/>
+      <c r="R7" s="50"/>
       <c r="T7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="16.5" x14ac:dyDescent="0.35">
@@ -883,58 +915,58 @@
         <v>1.8</v>
       </c>
       <c r="E8"/>
-      <c r="F8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>5</v>
+      <c r="F8" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>3</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V8" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="W8" s="18">
         <f>$B$3</f>
         <v>7.2</v>
       </c>
       <c r="X8" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="48"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="27">
         <v>39</v>
       </c>
@@ -942,36 +974,36 @@
         <v>1.5</v>
       </c>
       <c r="E9"/>
-      <c r="F9" s="40"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="10">
         <f>C$8*C9 + D$8*D9</f>
         <v>108.00000000000001</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="44">
         <f>F9+G9</f>
         <v>108.00000000000001</v>
       </c>
-      <c r="J9" s="45">
+      <c r="J9" s="43">
         <f>C9+D9</f>
         <v>40.5</v>
       </c>
-      <c r="K9" s="46">
+      <c r="K9" s="44">
         <f>$K$7*J9</f>
         <v>133.65</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="45">
         <f>G9/K9</f>
         <v>0.80808080808080818</v>
       </c>
       <c r="N9" s="25">
         <v>0.82</v>
       </c>
-      <c r="O9" s="46">
+      <c r="O9" s="44">
         <f>K9/N9</f>
         <v>162.98780487804879</v>
       </c>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="40"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="38"/>
       <c r="T9" s="10">
         <f>O9+R9</f>
         <v>162.98780487804879</v>
@@ -996,7 +1028,7 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="49"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="27">
         <v>16</v>
       </c>
@@ -1004,36 +1036,36 @@
         <v>1.5</v>
       </c>
       <c r="E10"/>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="10">
         <f t="shared" ref="G10:G12" si="0">C$8*C10 + D$8*D10</f>
         <v>45.900000000000006</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="33">
         <f t="shared" ref="H10:H12" si="1">F10+G10</f>
         <v>45.900000000000006</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="40">
         <f>C10+D10</f>
         <v>17.5</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="33">
         <f t="shared" ref="K10:K12" si="2">$K$7*J10</f>
         <v>57.75</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="41">
         <f t="shared" ref="L10:L12" si="3">G10/K10</f>
         <v>0.79480519480519496</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="31">
         <v>0.82</v>
       </c>
-      <c r="O10" s="34">
+      <c r="O10" s="33">
         <f t="shared" ref="O10:O12" si="4">K10/N10</f>
         <v>70.426829268292693</v>
       </c>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="41"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="39"/>
       <c r="T10" s="10">
         <f t="shared" ref="T10:T12" si="5">O10+R10</f>
         <v>70.426829268292693</v>
@@ -1055,9 +1087,9 @@
         <v>103.52743902439026</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B11" s="27">
         <v>220</v>
@@ -1077,33 +1109,33 @@
         <f t="shared" si="0"/>
         <v>59.400000000000006</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="33">
         <f t="shared" si="1"/>
         <v>1159.4000000000001</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="40">
         <f>C11+D11</f>
         <v>22.5</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="33">
         <f t="shared" si="2"/>
         <v>74.25</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="41">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="31">
         <v>0.83</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="33">
         <f t="shared" si="4"/>
         <v>89.457831325301214</v>
       </c>
-      <c r="Q11" s="32">
+      <c r="Q11" s="31">
         <v>0.94</v>
       </c>
-      <c r="R11" s="34">
+      <c r="R11" s="33">
         <f>F11/Q11</f>
         <v>1170.2127659574469</v>
       </c>
@@ -1127,9 +1159,9 @@
         <v>18.895058959241222</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B12" s="29">
         <v>380</v>
@@ -1161,7 +1193,7 @@
         <f t="shared" si="2"/>
         <v>100.64999999999999</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="42">
         <f t="shared" si="3"/>
         <v>0.80476900149031316</v>
       </c>
@@ -1224,9 +1256,9 @@
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
       <c r="V14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W14" s="50">
+        <v>19</v>
+      </c>
+      <c r="W14" s="48">
         <f>SUM(W9:W12)</f>
         <v>36.914850164008605</v>
       </c>
@@ -1237,23 +1269,33 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F7:H7"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="J6:L6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="F7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>